<commit_message>
add country partitioning to the narrative synthesis plot
</commit_message>
<xml_diff>
--- a/data/raw-data/international_policy_moments.xlsx
+++ b/data/raw-data/international_policy_moments.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>label</t>
   </si>
@@ -42,9 +43,6 @@
     <t>Kyoto Protocol</t>
   </si>
   <si>
-    <t>The first international treaty to set legally binding obligations on developed countries to reduce greenhouse gas emissions. It aimed to reduce emissions by an average of 5% below 1990 levels during the commitment period from 2008 to 2012. </t>
-  </si>
-  <si>
     <t>UNFCCC</t>
   </si>
   <si>
@@ -55,19 +53,124 @@
   </si>
   <si>
     <t>European Union’s ambitious roadmap to achieve climate neutrality by 2050</t>
+  </si>
+  <si>
+    <t>European 2030 climate &amp; energy framework</t>
+  </si>
+  <si>
+    <t>CDM</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The Clean Development Mechanism marked the uptick in carbon offsets (United Nations, 2018, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Achievements of the Clean Development Mechanism, harnessing incentive for climate action (2001–2018)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>EU policy on energy economy, targetting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> reducing greenhouse gas emissions and increasing use of renewable energies.</t>
+    </r>
+  </si>
+  <si>
+    <t>The economic shock instigated by the pandemic prompted regional and national policies to stimulate the economy and also deliver on climate mitigation commitments</t>
+  </si>
+  <si>
+    <t>Signing of the Kyoto Protocol: the first international treaty to set legally binding obligations on developed countries to reduce greenhouse gas emissions (eneterd into force in 2005)</t>
+  </si>
+  <si>
+    <t>plot</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>Financial crisis prompting green economic stimulus packages</t>
+  </si>
+  <si>
+    <t>2008/9 Financial crisis</t>
+  </si>
+  <si>
+    <t>COVID-19 pandemic</t>
+  </si>
+  <si>
+    <t>IMO efficiency policies</t>
+  </si>
+  <si>
+    <t>IPCC Special Reports</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF040C28"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,8 +193,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,15 +477,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -388,13 +493,16 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2015</v>
       </c>
@@ -402,27 +510,33 @@
         <v>2015</v>
       </c>
       <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2008</v>
-      </c>
-      <c r="B3">
-        <v>2012</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>1997</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1997</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1992</v>
       </c>
@@ -430,13 +544,16 @@
         <v>1992</v>
       </c>
       <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2019</v>
       </c>
@@ -444,14 +561,125 @@
         <v>2019</v>
       </c>
       <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2020</v>
+      </c>
+      <c r="B6">
+        <v>2020</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2014</v>
+      </c>
+      <c r="B7">
+        <v>2014</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
         <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2006</v>
+      </c>
+      <c r="B8">
+        <v>2006</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2008</v>
+      </c>
+      <c r="B9">
+        <v>2009</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2010</v>
+      </c>
+      <c r="B10">
+        <v>2013</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2018</v>
+      </c>
+      <c r="B11">
+        <v>2019</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>